<commit_message>
Implement json import and export
</commit_message>
<xml_diff>
--- a/SchoolManagementSystem/export/excel/giaovien.xlsx
+++ b/SchoolManagementSystem/export/excel/giaovien.xlsx
@@ -6,16 +6,13 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Teachers" r:id="rId3" sheetId="1"/>
+    <sheet name="giaovien.xlsx" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
-  <si>
-    <t/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>ID</t>
   </si>
@@ -23,7 +20,7 @@
     <t>Name</t>
   </si>
   <si>
-    <t>School ID</t>
+    <t>SchoolID</t>
   </si>
 </sst>
 </file>
@@ -83,18 +80,18 @@
   <cols>
     <col min="1" max="1" width="3.8515625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="8.25390625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="12.18359375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.55078125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="B1" t="s" s="1">
+      <c r="C1" t="s" s="1">
         <v>2</v>
-      </c>
-      <c r="C1" t="s" s="1">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>